<commit_message>
insert some comments and questions
</commit_message>
<xml_diff>
--- a/crosswalks/ALUM-IUCNGET/ALUMv8-IUCNGET.xlsx
+++ b/crosswalks/ALUM-IUCNGET/ALUMv8-IUCNGET.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C215534-B76D-48E8-81A8-13525A9E56B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289A0BFD-D55D-41F0-A1CE-188DFA234A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4935" yWindow="3240" windowWidth="17280" windowHeight="16200" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1395" yWindow="3900" windowWidth="17280" windowHeight="16200" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALUM V8" sheetId="5" r:id="rId1"/>
@@ -50,6 +50,24 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={7A7A686C-B1C4-45F8-B450-552E69DD158E}</author>
+  </authors>
+  <commentList>
+    <comment ref="C191" authorId="0" shapeId="0" xr:uid="{7A7A686C-B1C4-45F8-B450-552E69DD158E}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    One item per line please </t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>tc={0881399C-9480-46CC-A4A5-3D9FD195EE39}</author>
   </authors>
   <commentList>
@@ -68,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4350" uniqueCount="1045">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4370" uniqueCount="1052">
   <si>
     <t>Perennial horticulture</t>
   </si>
@@ -3401,12 +3419,33 @@
   <si>
     <t>mailto:Craig.Macfarlane@csiro.au</t>
   </si>
+  <si>
+    <t>Why not T7.3 here?</t>
+  </si>
+  <si>
+    <t>Why not T7.2 here?</t>
+  </si>
+  <si>
+    <t>Why not T7.1 here?</t>
+  </si>
+  <si>
+    <t>Why not T7.4 here?</t>
+  </si>
+  <si>
+    <t>Why not F3.1 here?</t>
+  </si>
+  <si>
+    <t>Why not F1 here?</t>
+  </si>
+  <si>
+    <t>Why not F3.5 here?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="50" x14ac:knownFonts="1">
+  <fonts count="51" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3721,6 +3760,12 @@
       <sz val="9"/>
       <color rgb="FF1F2328"/>
       <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -4049,7 +4094,7 @@
     <xf numFmtId="0" fontId="40" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4378,6 +4423,7 @@
     <xf numFmtId="0" fontId="27" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="41" fillId="12" borderId="0" xfId="5" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="40% - Accent4" xfId="2" builtinId="43"/>
@@ -4412,6 +4458,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4701,6 +4751,14 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C191" dT="2024-01-03T02:34:22.58" personId="{00000000-0000-0000-0000-000000000000}" id="{7A7A686C-B1C4-45F8-B450-552E69DD158E}">
+    <text xml:space="preserve">One item per line please </text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="G2" dT="2023-12-31T06:22:35.80" personId="{00000000-0000-0000-0000-000000000000}" id="{0881399C-9480-46CC-A4A5-3D9FD195EE39}">
     <text xml:space="preserve">An ORCID is preferred here. 
 I can see three Craig MacFarlane in ORCID but the details are hidden
@@ -19189,13 +19247,13 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:C196"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C193" sqref="C193"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E204" sqref="E204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19467,7 +19525,9 @@
       <c r="B25" s="116" t="s">
         <v>984</v>
       </c>
-      <c r="C25" s="135"/>
+      <c r="C25" s="162" t="s">
+        <v>1045</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -19520,7 +19580,9 @@
       <c r="B30" s="116" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="135"/>
+      <c r="C30" s="162" t="s">
+        <v>1046</v>
+      </c>
     </row>
     <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -19584,7 +19646,9 @@
       <c r="B36" s="116" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="135"/>
+      <c r="C36" s="162" t="s">
+        <v>1047</v>
+      </c>
     </row>
     <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -19681,7 +19745,9 @@
       <c r="B45" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="C45" s="135"/>
+      <c r="C45" s="162" t="s">
+        <v>1047</v>
+      </c>
     </row>
     <row r="46" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -19789,7 +19855,9 @@
       <c r="B55" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="C55" s="135"/>
+      <c r="C55" s="162" t="s">
+        <v>1047</v>
+      </c>
     </row>
     <row r="56" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
@@ -19895,7 +19963,9 @@
       <c r="B65" s="116" t="s">
         <v>985</v>
       </c>
-      <c r="C65" s="135"/>
+      <c r="C65" s="162" t="s">
+        <v>1045</v>
+      </c>
     </row>
     <row r="66" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
@@ -19948,7 +20018,9 @@
       <c r="B70" s="116" t="s">
         <v>504</v>
       </c>
-      <c r="C70" s="135"/>
+      <c r="C70" s="162" t="s">
+        <v>1046</v>
+      </c>
     </row>
     <row r="71" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
@@ -19994,14 +20066,13 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="116" t="s">
         <v>345</v>
       </c>
       <c r="B75" s="116" t="s">
         <v>29</v>
       </c>
-      <c r="C75" s="135"/>
     </row>
     <row r="76" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
@@ -20109,7 +20180,9 @@
       <c r="B85" s="116" t="s">
         <v>40</v>
       </c>
-      <c r="C85" s="135"/>
+      <c r="C85" s="162" t="s">
+        <v>1047</v>
+      </c>
     </row>
     <row r="86" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
@@ -20217,7 +20290,9 @@
       <c r="B95" s="116" t="s">
         <v>49</v>
       </c>
-      <c r="C95" s="135"/>
+      <c r="C95" s="162" t="s">
+        <v>1047</v>
+      </c>
     </row>
     <row r="96" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
@@ -20334,7 +20409,9 @@
       <c r="B106" s="116" t="s">
         <v>114</v>
       </c>
-      <c r="C106" s="135"/>
+      <c r="C106" s="162" t="s">
+        <v>1048</v>
+      </c>
     </row>
     <row r="107" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
@@ -20495,7 +20572,9 @@
       <c r="B121" s="116" t="s">
         <v>126</v>
       </c>
-      <c r="C121" s="135"/>
+      <c r="C121" s="162" t="s">
+        <v>1048</v>
+      </c>
     </row>
     <row r="122" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
@@ -20592,7 +20671,9 @@
       <c r="B130" s="116" t="s">
         <v>499</v>
       </c>
-      <c r="C130" s="135"/>
+      <c r="C130" s="162" t="s">
+        <v>1048</v>
+      </c>
     </row>
     <row r="131" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
@@ -20656,7 +20737,9 @@
       <c r="B136" s="116" t="s">
         <v>130</v>
       </c>
-      <c r="C136" s="135"/>
+      <c r="C136" s="162" t="s">
+        <v>1048</v>
+      </c>
     </row>
     <row r="137" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
@@ -20720,7 +20803,9 @@
       <c r="B142" s="116" t="s">
         <v>140</v>
       </c>
-      <c r="C142" s="135"/>
+      <c r="C142" s="162" t="s">
+        <v>1048</v>
+      </c>
     </row>
     <row r="143" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
@@ -20806,7 +20891,9 @@
       <c r="B150" s="116" t="s">
         <v>144</v>
       </c>
-      <c r="C150" s="135"/>
+      <c r="C150" s="162" t="s">
+        <v>1048</v>
+      </c>
     </row>
     <row r="151" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
@@ -20870,7 +20957,9 @@
       <c r="B156" s="116" t="s">
         <v>155</v>
       </c>
-      <c r="C156" s="135"/>
+      <c r="C156" s="162" t="s">
+        <v>1048</v>
+      </c>
     </row>
     <row r="157" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
@@ -20923,7 +21012,9 @@
       <c r="B161" s="116" t="s">
         <v>162</v>
       </c>
-      <c r="C161" s="135"/>
+      <c r="C161" s="162" t="s">
+        <v>1048</v>
+      </c>
     </row>
     <row r="162" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
@@ -21051,7 +21142,9 @@
       <c r="B173" s="116" t="s">
         <v>236</v>
       </c>
-      <c r="C173" s="135"/>
+      <c r="C173" s="162" t="s">
+        <v>1049</v>
+      </c>
     </row>
     <row r="174" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
@@ -21093,7 +21186,9 @@
       <c r="B177" s="116" t="s">
         <v>185</v>
       </c>
-      <c r="C177" s="137"/>
+      <c r="C177" s="162" t="s">
+        <v>1050</v>
+      </c>
     </row>
     <row r="178" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
@@ -21135,7 +21230,9 @@
       <c r="B181" s="116" t="s">
         <v>192</v>
       </c>
-      <c r="C181" s="135"/>
+      <c r="C181" s="162" t="s">
+        <v>1051</v>
+      </c>
     </row>
     <row r="182" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
@@ -21301,6 +21398,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -21309,7 +21407,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:J196"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:A196"/>
     </sheetView>
@@ -21992,11 +22090,11 @@
       </c>
       <c r="D25" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>get:groups/Why</v>
       </c>
       <c r="E25" t="str">
         <f>IF('ALUM_V8_vertical with IUCN'!C25=0,"",'ALUM_V8_vertical with IUCN'!C25)</f>
-        <v/>
+        <v>Why not T7.3 here?</v>
       </c>
       <c r="F25" s="150" t="s">
         <v>1043</v>
@@ -22139,11 +22237,11 @@
       </c>
       <c r="D30" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>get:groups/Why</v>
       </c>
       <c r="E30" t="str">
         <f>IF('ALUM_V8_vertical with IUCN'!C30=0,"",'ALUM_V8_vertical with IUCN'!C30)</f>
-        <v/>
+        <v>Why not T7.2 here?</v>
       </c>
       <c r="F30" s="150" t="s">
         <v>1043</v>
@@ -22316,11 +22414,11 @@
       </c>
       <c r="D36" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>get:groups/Why</v>
       </c>
       <c r="E36" t="str">
         <f>IF('ALUM_V8_vertical with IUCN'!C36=0,"",'ALUM_V8_vertical with IUCN'!C36)</f>
-        <v/>
+        <v>Why not T7.1 here?</v>
       </c>
       <c r="F36" s="150" t="s">
         <v>1043</v>
@@ -22583,11 +22681,11 @@
       </c>
       <c r="D45" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>get:groups/Why</v>
       </c>
       <c r="E45" t="str">
         <f>IF('ALUM_V8_vertical with IUCN'!C45=0,"",'ALUM_V8_vertical with IUCN'!C45)</f>
-        <v/>
+        <v>Why not T7.1 here?</v>
       </c>
       <c r="F45" s="150" t="s">
         <v>1043</v>
@@ -22880,11 +22978,11 @@
       </c>
       <c r="D55" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>get:groups/Why</v>
       </c>
       <c r="E55" t="str">
         <f>IF('ALUM_V8_vertical with IUCN'!C55=0,"",'ALUM_V8_vertical with IUCN'!C55)</f>
-        <v/>
+        <v>Why not T7.1 here?</v>
       </c>
       <c r="F55" s="150" t="s">
         <v>1043</v>
@@ -23159,11 +23257,11 @@
       </c>
       <c r="D65" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>get:groups/Why</v>
       </c>
       <c r="E65" t="str">
         <f>IF('ALUM_V8_vertical with IUCN'!C65=0,"",'ALUM_V8_vertical with IUCN'!C65)</f>
-        <v/>
+        <v>Why not T7.3 here?</v>
       </c>
       <c r="F65" s="150" t="s">
         <v>1043</v>
@@ -23306,11 +23404,11 @@
       </c>
       <c r="D70" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>get:groups/Why</v>
       </c>
       <c r="E70" t="str">
         <f>IF('ALUM_V8_vertical with IUCN'!C70=0,"",'ALUM_V8_vertical with IUCN'!C70)</f>
-        <v/>
+        <v>Why not T7.2 here?</v>
       </c>
       <c r="F70" s="150" t="s">
         <v>1043</v>
@@ -23453,11 +23551,11 @@
       </c>
       <c r="D75" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>get:groups/Why</v>
       </c>
       <c r="E75" t="str">
-        <f>IF('ALUM_V8_vertical with IUCN'!C75=0,"",'ALUM_V8_vertical with IUCN'!C75)</f>
-        <v/>
+        <f>IF('ALUM_V8_vertical with IUCN'!C95=0,"",'ALUM_V8_vertical with IUCN'!C95)</f>
+        <v>Why not T7.1 here?</v>
       </c>
       <c r="F75" s="150" t="s">
         <v>1043</v>
@@ -23750,11 +23848,11 @@
       </c>
       <c r="D85" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>get:groups/Why</v>
       </c>
       <c r="E85" t="str">
         <f>IF('ALUM_V8_vertical with IUCN'!C85=0,"",'ALUM_V8_vertical with IUCN'!C85)</f>
-        <v/>
+        <v>Why not T7.1 here?</v>
       </c>
       <c r="F85" s="150" t="s">
         <v>1043</v>
@@ -24049,9 +24147,9 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="E95" t="str">
-        <f>IF('ALUM_V8_vertical with IUCN'!C95=0,"",'ALUM_V8_vertical with IUCN'!C95)</f>
-        <v/>
+      <c r="E95" t="e">
+        <f>IF('ALUM_V8_vertical with IUCN'!#REF!=0,"",'ALUM_V8_vertical with IUCN'!#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="F95" s="150" t="s">
         <v>1043</v>
@@ -24356,11 +24454,11 @@
       </c>
       <c r="D106" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>get:groups/Why</v>
       </c>
       <c r="E106" t="str">
         <f>IF('ALUM_V8_vertical with IUCN'!C106=0,"",'ALUM_V8_vertical with IUCN'!C106)</f>
-        <v/>
+        <v>Why not T7.4 here?</v>
       </c>
       <c r="F106" s="150" t="s">
         <v>1043</v>
@@ -24800,11 +24898,11 @@
       </c>
       <c r="D121" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>get:groups/Why</v>
       </c>
       <c r="E121" t="str">
         <f>IF('ALUM_V8_vertical with IUCN'!C121=0,"",'ALUM_V8_vertical with IUCN'!C121)</f>
-        <v/>
+        <v>Why not T7.4 here?</v>
       </c>
       <c r="F121" s="150" t="s">
         <v>1043</v>
@@ -25067,11 +25165,11 @@
       </c>
       <c r="D130" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>get:groups/Why</v>
       </c>
       <c r="E130" t="str">
         <f>IF('ALUM_V8_vertical with IUCN'!C130=0,"",'ALUM_V8_vertical with IUCN'!C130)</f>
-        <v/>
+        <v>Why not T7.4 here?</v>
       </c>
       <c r="F130" s="150" t="s">
         <v>1043</v>
@@ -25244,11 +25342,11 @@
       </c>
       <c r="D136" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>get:groups/Why</v>
       </c>
       <c r="E136" t="str">
         <f>IF('ALUM_V8_vertical with IUCN'!C136=0,"",'ALUM_V8_vertical with IUCN'!C136)</f>
-        <v/>
+        <v>Why not T7.4 here?</v>
       </c>
       <c r="F136" s="150" t="s">
         <v>1043</v>
@@ -25421,11 +25519,11 @@
       </c>
       <c r="D142" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>get:groups/Why</v>
       </c>
       <c r="E142" t="str">
         <f>IF('ALUM_V8_vertical with IUCN'!C142=0,"",'ALUM_V8_vertical with IUCN'!C142)</f>
-        <v/>
+        <v>Why not T7.4 here?</v>
       </c>
       <c r="F142" s="150" t="s">
         <v>1043</v>
@@ -25658,11 +25756,11 @@
       </c>
       <c r="D150" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>get:groups/Why</v>
       </c>
       <c r="E150" t="str">
         <f>IF('ALUM_V8_vertical with IUCN'!C150=0,"",'ALUM_V8_vertical with IUCN'!C150)</f>
-        <v/>
+        <v>Why not T7.4 here?</v>
       </c>
       <c r="F150" s="150" t="s">
         <v>1043</v>
@@ -25835,11 +25933,11 @@
       </c>
       <c r="D156" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>get:groups/Why</v>
       </c>
       <c r="E156" t="str">
         <f>IF('ALUM_V8_vertical with IUCN'!C156=0,"",'ALUM_V8_vertical with IUCN'!C156)</f>
-        <v/>
+        <v>Why not T7.4 here?</v>
       </c>
       <c r="F156" s="150" t="s">
         <v>1043</v>
@@ -25982,11 +26080,11 @@
       </c>
       <c r="D161" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>get:groups/Why</v>
       </c>
       <c r="E161" t="str">
         <f>IF('ALUM_V8_vertical with IUCN'!C161=0,"",'ALUM_V8_vertical with IUCN'!C161)</f>
-        <v/>
+        <v>Why not T7.4 here?</v>
       </c>
       <c r="F161" s="150" t="s">
         <v>1043</v>
@@ -26336,11 +26434,11 @@
       </c>
       <c r="D173" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>get:groups/Why</v>
       </c>
       <c r="E173" t="str">
         <f>IF('ALUM_V8_vertical with IUCN'!C173=0,"",'ALUM_V8_vertical with IUCN'!C173)</f>
-        <v/>
+        <v>Why not F3.1 here?</v>
       </c>
       <c r="F173" s="150" t="s">
         <v>1043</v>
@@ -26453,11 +26551,11 @@
       </c>
       <c r="D177" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>get:biomes/Why</v>
       </c>
       <c r="E177" t="str">
         <f>IF('ALUM_V8_vertical with IUCN'!C177=0,"",'ALUM_V8_vertical with IUCN'!C177)</f>
-        <v/>
+        <v>Why not F1 here?</v>
       </c>
       <c r="F177" s="150" t="s">
         <v>1043</v>
@@ -26570,11 +26668,11 @@
       </c>
       <c r="D181" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>get:groups/Why</v>
       </c>
       <c r="E181" t="str">
         <f>IF('ALUM_V8_vertical with IUCN'!C181=0,"",'ALUM_V8_vertical with IUCN'!C181)</f>
-        <v/>
+        <v>Why not F3.5 here?</v>
       </c>
       <c r="F181" s="150" t="s">
         <v>1043</v>
@@ -27038,6 +27136,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DC29B5BE6945C34F8C7CB81794666E31" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9f7151ef105987b2d3758ef53560e213">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48c5b5cd9b8d25ff6dd15848836f4270" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -27169,15 +27276,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -27188,6 +27286,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEB67B5-0F24-4813-B2D2-A92E60BF00F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97EDE51C-194A-4D85-AD03-32004056A6AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27205,14 +27311,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEB67B5-0F24-4813-B2D2-A92E60BF00F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E64B25D3-7183-4323-848D-DB8D888013A0}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Changed zinc to Zinc.
</commit_message>
<xml_diff>
--- a/crosswalks/ALUM-IUCNGET/ALUMv8-IUCNGET.xlsx
+++ b/crosswalks/ALUM-IUCNGET/ALUMv8-IUCNGET.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289A0BFD-D55D-41F0-A1CE-188DFA234A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F48036-4A95-49E2-B4CC-B41E797D9D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="3900" windowWidth="17280" windowHeight="16200" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALUM V8" sheetId="5" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4370" uniqueCount="1052">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4370" uniqueCount="1053">
   <si>
     <t>Perennial horticulture</t>
   </si>
@@ -3440,6 +3440,9 @@
   <si>
     <t>Why not F3.5 here?</t>
   </si>
+  <si>
+    <t>Zinc</t>
+  </si>
 </sst>
 </file>
 
@@ -3449,6 +3452,13 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3760,12 +3770,6 @@
       <sz val="9"/>
       <color rgb="FF1F2328"/>
       <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -4084,17 +4088,17 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="38" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="39" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4103,193 +4107,202 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4297,16 +4310,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4315,115 +4319,116 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="40" fillId="12" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="39" fillId="11" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="38" fillId="10" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="41" fillId="14" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="37" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="42" fillId="18" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="43" fillId="14" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="45" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="41" fillId="12" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="40" fillId="11" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="39" fillId="10" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="42" fillId="14" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="43" fillId="18" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="44" fillId="14" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="46" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="47" fillId="17" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="46" fillId="16" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="38" fillId="10" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="48" fillId="17" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="47" fillId="16" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="39" fillId="10" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="12" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="18" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="18" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="12" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="40% - Accent4" xfId="2" builtinId="43"/>
@@ -4458,10 +4463,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4827,25 +4828,25 @@
     </row>
     <row r="2" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="152" t="s">
+      <c r="B2" s="153" t="s">
         <v>993</v>
       </c>
-      <c r="C2" s="152"/>
-      <c r="D2" s="152"/>
-      <c r="E2" s="152"/>
-      <c r="F2" s="152"/>
-      <c r="G2" s="152"/>
-      <c r="H2" s="152"/>
-      <c r="I2" s="152"/>
-      <c r="J2" s="152"/>
-      <c r="K2" s="152"/>
-      <c r="L2" s="152"/>
-      <c r="M2" s="152"/>
-      <c r="N2" s="152"/>
-      <c r="O2" s="152"/>
-      <c r="P2" s="152"/>
-      <c r="Q2" s="152"/>
-      <c r="R2" s="152"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
+      <c r="I2" s="153"/>
+      <c r="J2" s="153"/>
+      <c r="K2" s="153"/>
+      <c r="L2" s="153"/>
+      <c r="M2" s="153"/>
+      <c r="N2" s="153"/>
+      <c r="O2" s="153"/>
+      <c r="P2" s="153"/>
+      <c r="Q2" s="153"/>
+      <c r="R2" s="153"/>
       <c r="S2" s="2"/>
     </row>
     <row r="3" spans="1:25" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9933,8 +9934,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AX76"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AO2" sqref="AO2:AX41"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9971,25 +9972,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A1" s="153" t="s">
+      <c r="A1" s="154" t="s">
         <v>1005</v>
       </c>
-      <c r="B1" s="153"/>
-      <c r="C1" s="153"/>
-      <c r="D1" s="153"/>
-      <c r="E1" s="153"/>
-      <c r="F1" s="153"/>
-      <c r="G1" s="153"/>
-      <c r="H1" s="153"/>
-      <c r="I1" s="153"/>
-      <c r="J1" s="153"/>
-      <c r="K1" s="153"/>
-      <c r="O1" s="154" t="s">
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="154"/>
+      <c r="K1" s="154"/>
+      <c r="O1" s="155" t="s">
         <v>1005</v>
       </c>
-      <c r="P1" s="154"/>
-      <c r="Q1" s="154"/>
-      <c r="R1" s="154"/>
+      <c r="P1" s="155"/>
+      <c r="Q1" s="155"/>
+      <c r="R1" s="155"/>
       <c r="Y1" s="55"/>
       <c r="Z1" s="55"/>
       <c r="AA1" s="55"/>
@@ -10008,10 +10009,10 @@
       <c r="P2" s="126" t="s">
         <v>1007</v>
       </c>
-      <c r="Q2" s="154" t="s">
+      <c r="Q2" s="155" t="s">
         <v>951</v>
       </c>
-      <c r="R2" s="154"/>
+      <c r="R2" s="155"/>
       <c r="Y2" s="131" t="s">
         <v>960</v>
       </c>
@@ -10032,10 +10033,10 @@
       <c r="AO2" s="143" t="s">
         <v>960</v>
       </c>
-      <c r="AP2" s="156" t="s">
+      <c r="AP2" s="157" t="s">
         <v>1007</v>
       </c>
-      <c r="AQ2" s="156"/>
+      <c r="AQ2" s="157"/>
       <c r="AR2" s="144"/>
       <c r="AS2" s="144"/>
       <c r="AT2" s="145" t="s">
@@ -10102,10 +10103,10 @@
       <c r="AS3" s="141" t="s">
         <v>1009</v>
       </c>
-      <c r="AT3" s="155" t="s">
+      <c r="AT3" s="156" t="s">
         <v>946</v>
       </c>
-      <c r="AU3" s="155"/>
+      <c r="AU3" s="156"/>
       <c r="AV3" s="141" t="s">
         <v>947</v>
       </c>
@@ -10876,8 +10877,8 @@
         <v>808</v>
       </c>
       <c r="AD15" s="133"/>
-      <c r="AE15" s="133" t="s">
-        <v>953</v>
+      <c r="AE15" s="163" t="s">
+        <v>1052</v>
       </c>
       <c r="AO15" s="135" t="s">
         <v>528</v>
@@ -13295,13 +13296,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="157"/>
-      <c r="B1" s="158"/>
-      <c r="C1" s="159" t="s">
+      <c r="A1" s="158"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="160" t="s">
         <v>659</v>
       </c>
-      <c r="D1" s="160"/>
-      <c r="E1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="162"/>
     </row>
     <row r="2" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
@@ -18359,13 +18360,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="157"/>
-      <c r="B1" s="158"/>
-      <c r="C1" s="159" t="s">
+      <c r="A1" s="158"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="160" t="s">
         <v>659</v>
       </c>
-      <c r="D1" s="160"/>
-      <c r="E1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="162"/>
     </row>
     <row r="2" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="109" t="s">
@@ -19251,8 +19252,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:C196"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E204" sqref="E204"/>
     </sheetView>
   </sheetViews>
@@ -19525,7 +19526,7 @@
       <c r="B25" s="116" t="s">
         <v>984</v>
       </c>
-      <c r="C25" s="162" t="s">
+      <c r="C25" s="152" t="s">
         <v>1045</v>
       </c>
     </row>
@@ -19580,7 +19581,7 @@
       <c r="B30" s="116" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="162" t="s">
+      <c r="C30" s="152" t="s">
         <v>1046</v>
       </c>
     </row>
@@ -19646,7 +19647,7 @@
       <c r="B36" s="116" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="162" t="s">
+      <c r="C36" s="152" t="s">
         <v>1047</v>
       </c>
     </row>
@@ -19745,7 +19746,7 @@
       <c r="B45" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="C45" s="162" t="s">
+      <c r="C45" s="152" t="s">
         <v>1047</v>
       </c>
     </row>
@@ -19855,7 +19856,7 @@
       <c r="B55" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="C55" s="162" t="s">
+      <c r="C55" s="152" t="s">
         <v>1047</v>
       </c>
     </row>
@@ -19963,7 +19964,7 @@
       <c r="B65" s="116" t="s">
         <v>985</v>
       </c>
-      <c r="C65" s="162" t="s">
+      <c r="C65" s="152" t="s">
         <v>1045</v>
       </c>
     </row>
@@ -20018,7 +20019,7 @@
       <c r="B70" s="116" t="s">
         <v>504</v>
       </c>
-      <c r="C70" s="162" t="s">
+      <c r="C70" s="152" t="s">
         <v>1046</v>
       </c>
     </row>
@@ -20180,7 +20181,7 @@
       <c r="B85" s="116" t="s">
         <v>40</v>
       </c>
-      <c r="C85" s="162" t="s">
+      <c r="C85" s="152" t="s">
         <v>1047</v>
       </c>
     </row>
@@ -20290,7 +20291,7 @@
       <c r="B95" s="116" t="s">
         <v>49</v>
       </c>
-      <c r="C95" s="162" t="s">
+      <c r="C95" s="152" t="s">
         <v>1047</v>
       </c>
     </row>
@@ -20409,7 +20410,7 @@
       <c r="B106" s="116" t="s">
         <v>114</v>
       </c>
-      <c r="C106" s="162" t="s">
+      <c r="C106" s="152" t="s">
         <v>1048</v>
       </c>
     </row>
@@ -20572,7 +20573,7 @@
       <c r="B121" s="116" t="s">
         <v>126</v>
       </c>
-      <c r="C121" s="162" t="s">
+      <c r="C121" s="152" t="s">
         <v>1048</v>
       </c>
     </row>
@@ -20671,7 +20672,7 @@
       <c r="B130" s="116" t="s">
         <v>499</v>
       </c>
-      <c r="C130" s="162" t="s">
+      <c r="C130" s="152" t="s">
         <v>1048</v>
       </c>
     </row>
@@ -20737,7 +20738,7 @@
       <c r="B136" s="116" t="s">
         <v>130</v>
       </c>
-      <c r="C136" s="162" t="s">
+      <c r="C136" s="152" t="s">
         <v>1048</v>
       </c>
     </row>
@@ -20803,7 +20804,7 @@
       <c r="B142" s="116" t="s">
         <v>140</v>
       </c>
-      <c r="C142" s="162" t="s">
+      <c r="C142" s="152" t="s">
         <v>1048</v>
       </c>
     </row>
@@ -20891,7 +20892,7 @@
       <c r="B150" s="116" t="s">
         <v>144</v>
       </c>
-      <c r="C150" s="162" t="s">
+      <c r="C150" s="152" t="s">
         <v>1048</v>
       </c>
     </row>
@@ -20957,7 +20958,7 @@
       <c r="B156" s="116" t="s">
         <v>155</v>
       </c>
-      <c r="C156" s="162" t="s">
+      <c r="C156" s="152" t="s">
         <v>1048</v>
       </c>
     </row>
@@ -21012,7 +21013,7 @@
       <c r="B161" s="116" t="s">
         <v>162</v>
       </c>
-      <c r="C161" s="162" t="s">
+      <c r="C161" s="152" t="s">
         <v>1048</v>
       </c>
     </row>
@@ -21142,7 +21143,7 @@
       <c r="B173" s="116" t="s">
         <v>236</v>
       </c>
-      <c r="C173" s="162" t="s">
+      <c r="C173" s="152" t="s">
         <v>1049</v>
       </c>
     </row>
@@ -21186,7 +21187,7 @@
       <c r="B177" s="116" t="s">
         <v>185</v>
       </c>
-      <c r="C177" s="162" t="s">
+      <c r="C177" s="152" t="s">
         <v>1050</v>
       </c>
     </row>
@@ -21230,7 +21231,7 @@
       <c r="B181" s="116" t="s">
         <v>192</v>
       </c>
-      <c r="C181" s="162" t="s">
+      <c r="C181" s="152" t="s">
         <v>1051</v>
       </c>
     </row>
@@ -21409,7 +21410,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A196"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -27136,12 +27137,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -27277,18 +27278,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEB67B5-0F24-4813-B2D2-A92E60BF00F8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E64B25D3-7183-4323-848D-DB8D888013A0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -27312,11 +27315,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E64B25D3-7183-4323-848D-DB8D888013A0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEB67B5-0F24-4813-B2D2-A92E60BF00F8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added missing header to ALUM8-GET crosswalk.
</commit_message>
<xml_diff>
--- a/crosswalks/ALUM-IUCNGET/ALUMv8-IUCNGET.xlsx
+++ b/crosswalks/ALUM-IUCNGET/ALUMv8-IUCNGET.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FD8A66-6031-4C94-AD71-8C0CDF90D7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A19EDB2-93D5-4C32-879C-2C7EB35AE3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALUM V8" sheetId="5" r:id="rId1"/>
@@ -14,7 +14,8 @@
     <sheet name="commodities" sheetId="9" r:id="rId4"/>
     <sheet name="management" sheetId="10" r:id="rId5"/>
     <sheet name="ALUM_V8_vertical with IUCN" sheetId="11" r:id="rId6"/>
-    <sheet name="SSSOM" sheetId="14" r:id="rId7"/>
+    <sheet name="header" sheetId="15" r:id="rId7"/>
+    <sheet name="SSSOM" sheetId="14" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">commodities!$A$2:$F$268</definedName>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5223" uniqueCount="1222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5248" uniqueCount="1230">
   <si>
     <t>Perennial horticulture</t>
   </si>
@@ -3445,9 +3446,6 @@
     <t>Unclassified</t>
   </si>
   <si>
-    <t>FM1 Semi-confined transitional waters</t>
-  </si>
-  <si>
     <t>alum8:Strict-nature-reserves</t>
   </si>
   <si>
@@ -3928,17 +3926,51 @@
     <t>Insufficient information for classification</t>
   </si>
   <si>
-    <t>Will be mapped using NVIS dataset</t>
+    <t>creator_id: https://orcid.org/0000-0002-3884-3420</t>
+  </si>
+  <si>
+    <t>curie_map:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   get: https://global-ecosystems.org/explore/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   skos: http://www.w3.org/2004/02/skos/core#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   semapv: https://w3id.org/semapv/vocab/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   orcid: https://orcid.org/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   status: https://w3id.org/sssom/status/</t>
+  </si>
+  <si>
+    <t>license: https://creativecommons.org/publicdomain/zero/1.0/</t>
+  </si>
+  <si>
+    <t>alum8: TBA</t>
+  </si>
+  <si>
+    <t>mapping_set_id: http://w3id.org/env/crosswalk/alum82get/2024-05-09</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="52" x14ac:knownFonts="1">
+  <fonts count="53" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4579,19 +4611,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="39" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4600,193 +4633,202 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4794,16 +4836,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4812,119 +4845,120 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="41" fillId="12" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="40" fillId="11" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="39" fillId="10" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="42" fillId="14" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="38" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="43" fillId="18" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="44" fillId="14" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="46" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="42" fillId="12" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="41" fillId="11" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="40" fillId="10" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="43" fillId="14" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="39" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="44" fillId="18" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="45" fillId="14" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="47" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="48" fillId="17" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="47" fillId="16" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="39" fillId="10" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="49" fillId="17" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="48" fillId="16" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="40" fillId="10" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="42" fillId="12" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="12" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="18" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="18" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="40% - Accent4" xfId="2" builtinId="43"/>
     <cellStyle name="40% - Accent5" xfId="6" builtinId="47"/>
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -4932,8 +4966,16 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Neutral" xfId="5" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="7" xr:uid="{6E4AE3D0-7BAA-41EF-A73F-6403105D203D}"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -5014,10 +5056,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21949,13 +21987,85 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02CB4D65-9DAF-4373-8A3E-AE42C6AE42AD}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="104.140625" style="165" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="165"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="165" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="165" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="165" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="165" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="165" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="165" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="165" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="165" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="165" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="165" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28AAEF26-8574-478F-B8F3-4FDF27AEE69E}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:N164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L20" sqref="L20"/>
+      <selection pane="bottomLeft" activeCell="D159" sqref="D159:E164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -22018,7 +22128,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B2" t="s">
         <v>55</v>
@@ -22055,7 +22165,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B3" t="s">
         <v>57</v>
@@ -22092,7 +22202,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B4" t="s">
         <v>59</v>
@@ -22129,7 +22239,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="B5" t="s">
         <v>61</v>
@@ -22166,7 +22276,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B6" t="s">
         <v>63</v>
@@ -22203,7 +22313,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="B7" t="s">
         <v>65</v>
@@ -22240,7 +22350,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="B8" t="s">
         <v>67</v>
@@ -22277,7 +22387,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B9" t="s">
         <v>70</v>
@@ -22314,7 +22424,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="B10" t="s">
         <v>72</v>
@@ -22351,7 +22461,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="B11" t="s">
         <v>74</v>
@@ -22388,7 +22498,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="B12" t="s">
         <v>76</v>
@@ -22425,7 +22535,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B13" t="s">
         <v>1010</v>
@@ -22462,7 +22572,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="B14" t="s">
         <v>478</v>
@@ -22499,7 +22609,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="B15" t="s">
         <v>81</v>
@@ -22536,7 +22646,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B16" t="s">
         <v>391</v>
@@ -22566,14 +22676,14 @@
         <v>1055</v>
       </c>
       <c r="L16" t="s">
-        <v>1221</v>
+        <v>1057</v>
       </c>
       <c r="M16" s="154"/>
       <c r="N16" s="154"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="B17" t="s">
         <v>84</v>
@@ -22603,14 +22713,14 @@
         <v>1055</v>
       </c>
       <c r="L17" t="s">
-        <v>1221</v>
+        <v>1057</v>
       </c>
       <c r="M17" s="154"/>
       <c r="N17" s="154"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="B18" t="s">
         <v>991</v>
@@ -22640,14 +22750,14 @@
         <v>1055</v>
       </c>
       <c r="L18" t="s">
-        <v>1221</v>
+        <v>1057</v>
       </c>
       <c r="M18" s="154"/>
       <c r="N18" s="154"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B19" t="s">
         <v>233</v>
@@ -22677,14 +22787,14 @@
         <v>1055</v>
       </c>
       <c r="L19" t="s">
-        <v>1221</v>
+        <v>1057</v>
       </c>
       <c r="M19" s="154"/>
       <c r="N19" s="154"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B20" t="s">
         <v>986</v>
@@ -22719,7 +22829,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="B21" t="s">
         <v>989</v>
@@ -22754,7 +22864,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="B22" t="s">
         <v>482</v>
@@ -22789,7 +22899,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="B23" t="s">
         <v>483</v>
@@ -22824,7 +22934,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="B24" t="s">
         <v>95</v>
@@ -22859,7 +22969,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B25" t="s">
         <v>97</v>
@@ -22894,7 +23004,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B26" t="s">
         <v>385</v>
@@ -22929,7 +23039,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B27" t="s">
         <v>386</v>
@@ -22964,7 +23074,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="B28" t="s">
         <v>101</v>
@@ -22999,7 +23109,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B29" t="s">
         <v>104</v>
@@ -23034,7 +23144,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B30" t="s">
         <v>335</v>
@@ -23069,7 +23179,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="B31" t="s">
         <v>509</v>
@@ -23104,7 +23214,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B32" t="s">
         <v>558</v>
@@ -23139,7 +23249,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B33" t="s">
         <v>109</v>
@@ -23174,7 +23284,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B34" t="s">
         <v>111</v>
@@ -23209,7 +23319,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="B35" t="s">
         <v>431</v>
@@ -23244,7 +23354,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B36" t="s">
         <v>477</v>
@@ -23279,7 +23389,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B37" t="s">
         <v>2</v>
@@ -23314,7 +23424,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B38" t="s">
         <v>620</v>
@@ -23349,7 +23459,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
@@ -23384,7 +23494,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
@@ -23419,7 +23529,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B41" t="s">
         <v>627</v>
@@ -23454,7 +23564,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B42" t="s">
         <v>512</v>
@@ -23489,7 +23599,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B43" t="s">
         <v>514</v>
@@ -23524,7 +23634,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B44" t="s">
         <v>406</v>
@@ -23559,7 +23669,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B45" t="s">
         <v>438</v>
@@ -23594,7 +23704,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="B46" t="s">
         <v>484</v>
@@ -23629,7 +23739,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="B47" t="s">
         <v>516</v>
@@ -23664,7 +23774,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="B48" t="s">
         <v>518</v>
@@ -23699,7 +23809,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="B49" t="s">
         <v>394</v>
@@ -23729,14 +23839,14 @@
         <v>1055</v>
       </c>
       <c r="L49" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="M49" s="154"/>
       <c r="N49" s="154"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="B50" t="s">
         <v>395</v>
@@ -23766,14 +23876,14 @@
         <v>1055</v>
       </c>
       <c r="L50" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="M50" s="154"/>
       <c r="N50" s="154"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B51" t="s">
         <v>396</v>
@@ -23803,14 +23913,14 @@
         <v>1055</v>
       </c>
       <c r="L51" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="M51" s="154"/>
       <c r="N51" s="154"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="B52" t="s">
         <v>397</v>
@@ -23840,14 +23950,14 @@
         <v>1055</v>
       </c>
       <c r="L52" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="M52" s="154"/>
       <c r="N52" s="154"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="B53" t="s">
         <v>445</v>
@@ -23877,14 +23987,14 @@
         <v>1055</v>
       </c>
       <c r="L53" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="M53" s="154"/>
       <c r="N53" s="154"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="B54" t="s">
         <v>987</v>
@@ -23919,7 +24029,7 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="B55" t="s">
         <v>990</v>
@@ -23954,7 +24064,7 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B56" t="s">
         <v>488</v>
@@ -23989,7 +24099,7 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B57" t="s">
         <v>505</v>
@@ -24024,7 +24134,7 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="B58" t="s">
         <v>22</v>
@@ -24059,7 +24169,7 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B59" t="s">
         <v>24</v>
@@ -24094,7 +24204,7 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B60" t="s">
         <v>26</v>
@@ -24129,7 +24239,7 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B61" t="s">
         <v>28</v>
@@ -24164,7 +24274,7 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B62" t="s">
         <v>31</v>
@@ -24199,7 +24309,7 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="B63" t="s">
         <v>507</v>
@@ -24234,7 +24344,7 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B64" t="s">
         <v>508</v>
@@ -24269,7 +24379,7 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="B65" t="s">
         <v>655</v>
@@ -24304,7 +24414,7 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B66" t="s">
         <v>36</v>
@@ -24339,7 +24449,7 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B67" t="s">
         <v>38</v>
@@ -24374,7 +24484,7 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="B68" t="s">
         <v>489</v>
@@ -24409,7 +24519,7 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B69" t="s">
         <v>490</v>
@@ -24444,7 +24554,7 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="B70" t="s">
         <v>464</v>
@@ -24479,7 +24589,7 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="B71" t="s">
         <v>42</v>
@@ -24514,7 +24624,7 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="B72" t="s">
         <v>621</v>
@@ -24549,7 +24659,7 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="B73" t="s">
         <v>46</v>
@@ -24584,7 +24694,7 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="B74" t="s">
         <v>48</v>
@@ -24619,7 +24729,7 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="B75" t="s">
         <v>653</v>
@@ -24654,7 +24764,7 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="B76" t="s">
         <v>513</v>
@@ -24689,7 +24799,7 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="B77" t="s">
         <v>515</v>
@@ -24724,7 +24834,7 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B78" t="s">
         <v>405</v>
@@ -24759,7 +24869,7 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="B79" t="s">
         <v>437</v>
@@ -24794,7 +24904,7 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="B80" t="s">
         <v>491</v>
@@ -24829,7 +24939,7 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="B81" t="s">
         <v>517</v>
@@ -24864,7 +24974,7 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="B82" t="s">
         <v>519</v>
@@ -24899,7 +25009,7 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="B83" t="s">
         <v>404</v>
@@ -24934,7 +25044,7 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="B84" t="s">
         <v>398</v>
@@ -24964,14 +25074,14 @@
         <v>1055</v>
       </c>
       <c r="L84" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="M84" s="154"/>
       <c r="N84" s="154"/>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="B85" t="s">
         <v>399</v>
@@ -25001,14 +25111,14 @@
         <v>1055</v>
       </c>
       <c r="L85" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="M85" s="154"/>
       <c r="N85" s="154"/>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="B86" t="s">
         <v>400</v>
@@ -25038,14 +25148,14 @@
         <v>1055</v>
       </c>
       <c r="L86" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="M86" s="154"/>
       <c r="N86" s="154"/>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="B87" t="s">
         <v>992</v>
@@ -25075,14 +25185,14 @@
         <v>1055</v>
       </c>
       <c r="L87" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="M87" s="154"/>
       <c r="N87" s="154"/>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="B88" t="s">
         <v>449</v>
@@ -25112,14 +25222,14 @@
         <v>1055</v>
       </c>
       <c r="L88" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="M88" s="154"/>
       <c r="N88" s="154"/>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B89" t="s">
         <v>597</v>
@@ -25154,7 +25264,7 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B90" t="s">
         <v>116</v>
@@ -25189,7 +25299,7 @@
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="B91" t="s">
         <v>118</v>
@@ -25224,7 +25334,7 @@
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B92" t="s">
         <v>982</v>
@@ -25259,7 +25369,7 @@
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="B93" t="s">
         <v>451</v>
@@ -25294,7 +25404,7 @@
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B94" t="s">
         <v>494</v>
@@ -25329,7 +25439,7 @@
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="B95" t="s">
         <v>521</v>
@@ -25364,7 +25474,7 @@
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B96" t="s">
         <v>497</v>
@@ -25399,7 +25509,7 @@
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B97" t="s">
         <v>498</v>
@@ -25434,7 +25544,7 @@
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B98" t="s">
         <v>235</v>
@@ -25469,7 +25579,7 @@
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B99" t="s">
         <v>465</v>
@@ -25504,7 +25614,7 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B100" t="s">
         <v>656</v>
@@ -25539,7 +25649,7 @@
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="B101" t="s">
         <v>524</v>
@@ -25574,7 +25684,7 @@
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B102" t="s">
         <v>448</v>
@@ -25609,7 +25719,7 @@
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="B103" t="s">
         <v>408</v>
@@ -25644,7 +25754,7 @@
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="B104" t="s">
         <v>410</v>
@@ -25679,7 +25789,7 @@
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="B105" t="s">
         <v>412</v>
@@ -25714,7 +25824,7 @@
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="B106" t="s">
         <v>415</v>
@@ -25749,7 +25859,7 @@
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="B107" t="s">
         <v>418</v>
@@ -25784,7 +25894,7 @@
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="B108" t="s">
         <v>423</v>
@@ -25819,7 +25929,7 @@
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="B109" t="s">
         <v>419</v>
@@ -25854,7 +25964,7 @@
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="B110" t="s">
         <v>128</v>
@@ -25889,7 +25999,7 @@
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="B111" t="s">
         <v>500</v>
@@ -25924,7 +26034,7 @@
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="B112" t="s">
         <v>501</v>
@@ -25959,7 +26069,7 @@
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="B113" t="s">
         <v>454</v>
@@ -25994,7 +26104,7 @@
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="B114" t="s">
         <v>443</v>
@@ -26029,7 +26139,7 @@
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="B115" t="s">
         <v>132</v>
@@ -26064,7 +26174,7 @@
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="B116" t="s">
         <v>134</v>
@@ -26099,7 +26209,7 @@
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="B117" t="s">
         <v>136</v>
@@ -26134,7 +26244,7 @@
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="B118" t="s">
         <v>502</v>
@@ -26169,7 +26279,7 @@
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="B119" t="s">
         <v>139</v>
@@ -26204,7 +26314,7 @@
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B120" t="s">
         <v>424</v>
@@ -26239,7 +26349,7 @@
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="B121" t="s">
         <v>426</v>
@@ -26274,7 +26384,7 @@
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="B122" t="s">
         <v>654</v>
@@ -26309,7 +26419,7 @@
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="B123" t="s">
         <v>526</v>
@@ -26344,7 +26454,7 @@
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="B124" t="s">
         <v>430</v>
@@ -26379,7 +26489,7 @@
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="B125" t="s">
         <v>143</v>
@@ -26414,7 +26524,7 @@
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="B126" t="s">
         <v>463</v>
@@ -26449,7 +26559,7 @@
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="B127" t="s">
         <v>146</v>
@@ -26484,7 +26594,7 @@
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="B128" t="s">
         <v>148</v>
@@ -26519,7 +26629,7 @@
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B129" t="s">
         <v>150</v>
@@ -26554,7 +26664,7 @@
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="B130" t="s">
         <v>152</v>
@@ -26589,7 +26699,7 @@
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="B131" t="s">
         <v>154</v>
@@ -26624,7 +26734,7 @@
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="B132" t="s">
         <v>157</v>
@@ -26659,7 +26769,7 @@
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="B133" t="s">
         <v>159</v>
@@ -26694,7 +26804,7 @@
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="B134" t="s">
         <v>161</v>
@@ -26729,7 +26839,7 @@
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B135" t="s">
         <v>522</v>
@@ -26764,7 +26874,7 @@
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="B136" t="s">
         <v>184</v>
@@ -26799,7 +26909,7 @@
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="B137" t="s">
         <v>166</v>
@@ -26834,7 +26944,7 @@
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B138" t="s">
         <v>168</v>
@@ -26869,7 +26979,7 @@
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="B139" t="s">
         <v>170</v>
@@ -26904,7 +27014,7 @@
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="B140" t="s">
         <v>506</v>
@@ -26939,7 +27049,7 @@
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="B141" t="s">
         <v>174</v>
@@ -26947,12 +27057,11 @@
       <c r="C141" t="s">
         <v>1040</v>
       </c>
-      <c r="D141" t="str">
-        <f t="shared" si="2"/>
-        <v>get:biomes/F2</v>
-      </c>
-      <c r="E141" t="s">
-        <v>1024</v>
+      <c r="D141" s="104" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E141" s="104" t="s">
+        <v>1059</v>
       </c>
       <c r="F141" s="150" t="s">
         <v>1043</v>
@@ -26977,7 +27086,7 @@
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="B142" t="s">
         <v>176</v>
@@ -26985,12 +27094,11 @@
       <c r="C142" t="s">
         <v>1040</v>
       </c>
-      <c r="D142" t="str">
-        <f t="shared" si="2"/>
-        <v>get:biomes/F2</v>
-      </c>
-      <c r="E142" t="s">
-        <v>1024</v>
+      <c r="D142" s="104" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E142" s="104" t="s">
+        <v>1059</v>
       </c>
       <c r="F142" s="150" t="s">
         <v>1043</v>
@@ -27015,7 +27123,7 @@
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="B143" t="s">
         <v>178</v>
@@ -27023,12 +27131,11 @@
       <c r="C143" t="s">
         <v>1040</v>
       </c>
-      <c r="D143" t="str">
-        <f t="shared" si="2"/>
-        <v>get:biomes/F2</v>
-      </c>
-      <c r="E143" t="s">
-        <v>1024</v>
+      <c r="D143" s="104" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E143" s="104" t="s">
+        <v>1059</v>
       </c>
       <c r="F143" s="150" t="s">
         <v>1043</v>
@@ -27053,7 +27160,7 @@
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B144" t="s">
         <v>457</v>
@@ -27088,7 +27195,7 @@
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B145" t="s">
         <v>457</v>
@@ -27123,7 +27230,7 @@
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="B146" t="s">
         <v>179</v>
@@ -27158,7 +27265,7 @@
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="B147" t="s">
         <v>387</v>
@@ -27193,7 +27300,7 @@
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="B148" t="s">
         <v>183</v>
@@ -27228,7 +27335,7 @@
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="B149" t="s">
         <v>187</v>
@@ -27236,12 +27343,11 @@
       <c r="C149" t="s">
         <v>1040</v>
       </c>
-      <c r="D149" t="str">
-        <f t="shared" si="2"/>
-        <v>get:biomes/F1</v>
-      </c>
-      <c r="E149" t="s">
-        <v>1021</v>
+      <c r="D149" s="104" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E149" s="104" t="s">
+        <v>1059</v>
       </c>
       <c r="F149" s="150" t="s">
         <v>1043</v>
@@ -27266,7 +27372,7 @@
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="B150" t="s">
         <v>189</v>
@@ -27274,12 +27380,11 @@
       <c r="C150" t="s">
         <v>1040</v>
       </c>
-      <c r="D150" t="str">
-        <f t="shared" si="2"/>
-        <v>get:biomes/F1</v>
-      </c>
-      <c r="E150" t="s">
-        <v>1021</v>
+      <c r="D150" s="104" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E150" s="104" t="s">
+        <v>1059</v>
       </c>
       <c r="F150" s="150" t="s">
         <v>1043</v>
@@ -27304,7 +27409,7 @@
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="B151" t="s">
         <v>191</v>
@@ -27312,12 +27417,11 @@
       <c r="C151" t="s">
         <v>1040</v>
       </c>
-      <c r="D151" t="str">
-        <f t="shared" si="2"/>
-        <v>get:biomes/F1</v>
-      </c>
-      <c r="E151" t="s">
-        <v>1021</v>
+      <c r="D151" s="104" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E151" s="104" t="s">
+        <v>1059</v>
       </c>
       <c r="F151" s="150" t="s">
         <v>1043</v>
@@ -27342,7 +27446,7 @@
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="B152" t="s">
         <v>194</v>
@@ -27377,7 +27481,7 @@
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="B153" t="s">
         <v>196</v>
@@ -27412,7 +27516,7 @@
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="B154" t="s">
         <v>164</v>
@@ -27447,7 +27551,7 @@
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B155" t="s">
         <v>199</v>
@@ -27455,12 +27559,11 @@
       <c r="C155" t="s">
         <v>1040</v>
       </c>
-      <c r="D155" t="str">
-        <f t="shared" si="2"/>
-        <v>get:biomes/TF1</v>
-      </c>
-      <c r="E155" t="s">
-        <v>1035</v>
+      <c r="D155" s="104" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E155" s="104" t="s">
+        <v>1059</v>
       </c>
       <c r="F155" s="150" t="s">
         <v>1043</v>
@@ -27485,7 +27588,7 @@
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="B156" t="s">
         <v>201</v>
@@ -27493,12 +27596,11 @@
       <c r="C156" t="s">
         <v>1040</v>
       </c>
-      <c r="D156" t="str">
-        <f t="shared" si="2"/>
-        <v>get:biomes/TF1</v>
-      </c>
-      <c r="E156" t="s">
-        <v>1035</v>
+      <c r="D156" s="104" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E156" s="104" t="s">
+        <v>1059</v>
       </c>
       <c r="F156" s="150" t="s">
         <v>1043</v>
@@ -27523,7 +27625,7 @@
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="B157" t="s">
         <v>203</v>
@@ -27531,12 +27633,11 @@
       <c r="C157" t="s">
         <v>1040</v>
       </c>
-      <c r="D157" t="str">
-        <f t="shared" si="2"/>
-        <v>get:biomes/TF1</v>
-      </c>
-      <c r="E157" t="s">
-        <v>1035</v>
+      <c r="D157" s="104" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E157" s="104" t="s">
+        <v>1059</v>
       </c>
       <c r="F157" s="150" t="s">
         <v>1043</v>
@@ -27561,7 +27662,7 @@
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B158" t="s">
         <v>459</v>
@@ -27596,7 +27697,7 @@
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B159" t="s">
         <v>206</v>
@@ -27604,12 +27705,11 @@
       <c r="C159" s="104" t="s">
         <v>1040</v>
       </c>
-      <c r="D159" t="str">
-        <f t="shared" si="2"/>
-        <v>get:biomes/FM1</v>
+      <c r="D159" s="104" t="s">
+        <v>1058</v>
       </c>
       <c r="E159" s="104" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="F159" s="150" t="s">
         <v>1043</v>
@@ -27634,7 +27734,7 @@
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B160" t="s">
         <v>206</v>
@@ -27642,12 +27742,11 @@
       <c r="C160" s="104" t="s">
         <v>1040</v>
       </c>
-      <c r="D160" t="str">
-        <f t="shared" ref="D160:D164" si="3">(IF(LEN(A160),IF(ISNUMBER(SEARCH(" ",E160)),IF(ISNUMBER(SEARCH(".",E160)),_xlfn.CONCAT("get:groups/",LEFT(E160,FIND(" ",E160)-1)),_xlfn.CONCAT("get:biomes/",LEFT(E160,FIND(" ",E160)-1))),"")))</f>
-        <v>get:biomes/FM1</v>
+      <c r="D160" s="104" t="s">
+        <v>1058</v>
       </c>
       <c r="E160" s="104" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="F160" s="150" t="s">
         <v>1043</v>
@@ -27672,7 +27771,7 @@
     </row>
     <row r="161" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="B161" t="s">
         <v>208</v>
@@ -27680,12 +27779,11 @@
       <c r="C161" s="104" t="s">
         <v>1040</v>
       </c>
-      <c r="D161" t="str">
-        <f t="shared" si="3"/>
-        <v>get:biomes/FM1</v>
+      <c r="D161" s="104" t="s">
+        <v>1058</v>
       </c>
       <c r="E161" s="104" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="F161" s="150" t="s">
         <v>1043</v>
@@ -27710,7 +27808,7 @@
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="B162" t="s">
         <v>208</v>
@@ -27718,12 +27816,11 @@
       <c r="C162" s="104" t="s">
         <v>1040</v>
       </c>
-      <c r="D162" t="str">
-        <f t="shared" si="3"/>
-        <v>get:biomes/FM1</v>
+      <c r="D162" s="104" t="s">
+        <v>1058</v>
       </c>
       <c r="E162" s="104" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="F162" s="150" t="s">
         <v>1043</v>
@@ -27748,7 +27845,7 @@
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="B163" t="s">
         <v>210</v>
@@ -27756,12 +27853,11 @@
       <c r="C163" s="104" t="s">
         <v>1040</v>
       </c>
-      <c r="D163" t="str">
-        <f t="shared" si="3"/>
-        <v>get:biomes/FM1</v>
+      <c r="D163" s="104" t="s">
+        <v>1058</v>
       </c>
       <c r="E163" s="104" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="F163" s="150" t="s">
         <v>1043</v>
@@ -27786,7 +27882,7 @@
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="B164" t="s">
         <v>210</v>
@@ -27794,12 +27890,11 @@
       <c r="C164" s="104" t="s">
         <v>1040</v>
       </c>
-      <c r="D164" t="str">
-        <f t="shared" si="3"/>
-        <v>get:biomes/FM1</v>
+      <c r="D164" s="104" t="s">
+        <v>1058</v>
       </c>
       <c r="E164" s="104" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="F164" s="150" t="s">
         <v>1043</v>
@@ -27823,44 +27918,49 @@
       <c r="N164" s="154"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C159:C164 E159:E164 C2:E13">
-    <cfRule type="containsBlanks" dxfId="7" priority="8">
+  <conditionalFormatting sqref="C159:C164">
+    <cfRule type="containsBlanks" dxfId="8" priority="12">
+      <formula>LEN(TRIM(C159))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:E19">
+    <cfRule type="containsBlanks" dxfId="7" priority="5">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:E15">
+  <conditionalFormatting sqref="C49:E53">
     <cfRule type="containsBlanks" dxfId="6" priority="7">
-      <formula>LEN(TRIM(C15))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C160:E160">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(C160))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C161:E164">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
-      <formula>LEN(TRIM(C161))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14:E14">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(C14))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:E53">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(C49))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C84:E88">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
       <formula>LEN(TRIM(C84))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C16:E19">
+  <conditionalFormatting sqref="C160:C164">
+    <cfRule type="containsBlanks" dxfId="4" priority="9">
+      <formula>LEN(TRIM(C160))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D141:E143">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(D141))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D149:E151">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(D149))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D155:E157">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(D155))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D159:E164">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(C16))=0</formula>
+      <formula>LEN(TRIM(D159))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -27869,6 +27969,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DC29B5BE6945C34F8C7CB81794666E31" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9f7151ef105987b2d3758ef53560e213">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48c5b5cd9b8d25ff6dd15848836f4270" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -28000,15 +28109,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -28019,6 +28119,16 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E64B25D3-7183-4323-848D-DB8D888013A0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97EDE51C-194A-4D85-AD03-32004056A6AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28036,16 +28146,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E64B25D3-7183-4323-848D-DB8D888013A0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEB67B5-0F24-4813-B2D2-A92E60BF00F8}">
   <ds:schemaRefs>

</xml_diff>